<commit_message>
Maven Code Merge Changes-9/19/2017
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite StatutoryAdoptionPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite StatutoryAdoptionPay201718.xlsx
@@ -4,28 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="9" firstSheet="8" windowHeight="5400" windowWidth="15168" xWindow="384" yWindow="36"/>
+    <workbookView xWindow="384" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="ResetData" r:id="rId2" sheetId="14"/>
-    <sheet name="CreateFemaleEmployee" r:id="rId3" sheetId="2"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="6"/>
-    <sheet name="SmallEmployerRelief" r:id="rId5" sheetId="3"/>
-    <sheet name="ProcessPayrollForJuneMonthSAP" r:id="rId6" sheetId="7"/>
-    <sheet name="ProcessPayrollForJulyMonthSAP" r:id="rId7" sheetId="8"/>
-    <sheet name="ProcessPayrollForAugustMonthSAP" r:id="rId8" sheetId="9"/>
-    <sheet name="CreateLeaveRequest" r:id="rId9" sheetId="10"/>
-    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="11"/>
-    <sheet name="ProcessPayrollForDecMonthSAP" r:id="rId11" sheetId="12"/>
-    <sheet name="ProcessPayrollForJan2016MontSAP" r:id="rId12" sheetId="13"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetData" sheetId="14" r:id="rId2"/>
+    <sheet name="CreateFemaleEmployee" sheetId="2" r:id="rId3"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="6" r:id="rId4"/>
+    <sheet name="SmallEmployerRelief" sheetId="3" r:id="rId5"/>
+    <sheet name="ProcessPayrollForJuneMonthSAP" sheetId="7" r:id="rId6"/>
+    <sheet name="ProcessPayrollForJulyMonthSAP" sheetId="8" r:id="rId7"/>
+    <sheet name="ProcessPayrollForAugustMonthSAP" sheetId="9" r:id="rId8"/>
+    <sheet name="CreateLeaveRequest" sheetId="10" r:id="rId9"/>
+    <sheet name="AverageWeeklyEarningsTestReport" sheetId="11" r:id="rId10"/>
+    <sheet name="ProcessPayrollForDecMonthSAP" sheetId="12" r:id="rId11"/>
+    <sheet name="ProcessPayrollForJan2016MontSAP" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="190">
   <si>
     <t>TC</t>
   </si>
@@ -666,63 +666,63 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -736,10 +736,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -897,7 +897,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -906,13 +906,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -922,7 +922,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -931,7 +931,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -940,7 +940,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -950,12 +950,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -986,7 +986,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1005,7 +1005,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1029,7 +1029,7 @@
     <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="44.33203125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.11328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.04052734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="28.8" r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>118</v>
       </c>
     </row>
-    <row ht="28.8" r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="28.8" r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>150</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="28.8" r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -1285,12 +1285,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1354,7 +1354,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="74.400000000000006" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -1391,12 +1391,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1460,7 +1460,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -1499,12 +1499,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1569,7 +1569,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -1608,12 +1608,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1646,7 +1646,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="21.6" r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>116</v>
       </c>
@@ -1661,12 +1661,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2067,15 +2067,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId3" ref="C2"/>
-    <hyperlink r:id="rId4" ref="D2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2115,7 +2115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>116</v>
       </c>
@@ -2136,12 +2136,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2171,7 +2171,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="17.399999999999999" r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>116</v>
       </c>
@@ -2183,13 +2183,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2255,7 +2255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -2294,12 +2294,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2364,7 +2364,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -2403,12 +2403,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2472,7 +2472,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -2511,12 +2511,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2607,6 +2607,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>